<commit_message>
Updated and created test cases document
</commit_message>
<xml_diff>
--- a/Templates/Test Cases (template).xlsx
+++ b/Templates/Test Cases (template).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donna Turner\ShareFile\Personal Folders\BCIT\Comp3900 - 201830\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jango\Documents\SMP\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CECAD485-6502-4D66-A1AE-B4552C7AC874}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7411CD1E-5D1F-4E42-8505-51F0A4E0ED94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="7833" activeTab="1" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -252,6 +252,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,17 +576,17 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3515625" customWidth="1"/>
-    <col min="2" max="2" width="27.76171875" customWidth="1"/>
-    <col min="3" max="3" width="14.76171875" customWidth="1"/>
-    <col min="4" max="4" width="23.5859375" customWidth="1"/>
-    <col min="5" max="5" width="19.41015625" customWidth="1"/>
-    <col min="6" max="6" width="13.9375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -591,7 +594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -601,7 +604,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -619,7 +622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -637,7 +640,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -655,7 +658,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -675,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -695,7 +698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -705,7 +708,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -715,7 +718,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -733,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -751,7 +754,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -769,7 +772,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -789,7 +792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -809,7 +812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -830,39 +833,42 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3515625" customWidth="1"/>
-    <col min="2" max="2" width="27.76171875" customWidth="1"/>
-    <col min="3" max="3" width="14.76171875" customWidth="1"/>
-    <col min="4" max="4" width="23.5859375" customWidth="1"/>
-    <col min="5" max="5" width="19.41015625" customWidth="1"/>
-    <col min="6" max="6" width="13.9375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.52734375" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.6">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+      <c r="E1" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -883,7 +889,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -901,7 +907,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -919,7 +925,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -942,7 +948,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -962,7 +968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -972,17 +978,17 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.6">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1018,7 +1024,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1036,7 +1042,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1087,6 +1093,12 @@
       <c r="F17" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Settings stuff in php & supervisor minutes
</commit_message>
<xml_diff>
--- a/Templates/Test Cases (template).xlsx
+++ b/Templates/Test Cases (template).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jango\Documents\SMP\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Documents\Super Points repo\SMP\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7411CD1E-5D1F-4E42-8505-51F0A4E0ED94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0D0F90-C591-443C-8E48-F8B0F053EB2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="24">
   <si>
     <t>Input</t>
   </si>
@@ -151,6 +151,23 @@
   </si>
   <si>
     <t>DD Month YYYY, fixed by TeamMember1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scenario: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#1,  New business, upload promotion w/ Image</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -576,17 +593,17 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -594,7 +611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -604,7 +621,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -622,7 +639,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -640,7 +657,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -658,7 +675,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -678,7 +695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -698,7 +715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -708,7 +725,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -718,7 +735,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -736,7 +753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -754,7 +771,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -772,7 +789,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -792,7 +809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -812,7 +829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -833,21 +850,21 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
@@ -858,17 +875,17 @@
       </c>
       <c r="E1" s="10"/>
     </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -889,7 +906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -907,7 +924,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -925,7 +942,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -948,7 +965,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -968,7 +985,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -978,7 +995,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
@@ -988,7 +1005,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1024,7 +1041,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1042,7 +1059,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1062,7 +1079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -1082,7 +1099,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1093,11 +1110,12 @@
       <c r="F17" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>